<commit_message>
bd: update db, end creating data for import
</commit_message>
<xml_diff>
--- a/database/data_for_import/План - три месяца (1).xlsx
+++ b/database/data_for_import/План - три месяца (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\pp+diplom\study_1c\database\data_for_import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Progects\study_1c\database\data_for_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E163ED4A-6010-4889-A8B1-959623ADEB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F3BC88-3FF7-45E7-ADFB-8101CA781A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="866" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="866" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Начни тут!" sheetId="1" r:id="rId1"/>
@@ -2134,11 +2134,19 @@
     <numFmt numFmtId="164" formatCode="dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3510,752 +3518,752 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="276">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="28" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="28" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="28" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="27" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="30" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="64" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="28" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="7" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="6" borderId="30" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="6" borderId="64" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="7" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4999,7 +5007,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="222" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -5008,7 +5016,7 @@
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="219"/>
+      <c r="B2" s="222"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5018,14 +5026,14 @@
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="220"/>
+      <c r="C3" s="223"/>
     </row>
     <row r="4" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="220"/>
+      <c r="C4" s="223"/>
     </row>
     <row r="5" spans="1:3" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -5046,7 +5054,7 @@
       <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="220"/>
+      <c r="C7" s="223"/>
     </row>
     <row r="8" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -5055,7 +5063,7 @@
       <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="220"/>
+      <c r="C8" s="223"/>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
@@ -5064,7 +5072,7 @@
       <c r="B9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="220"/>
+      <c r="C9" s="223"/>
     </row>
     <row r="10" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
@@ -5073,7 +5081,7 @@
       <c r="B10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="220"/>
+      <c r="C10" s="223"/>
     </row>
     <row r="11" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
@@ -5082,23 +5090,23 @@
       <c r="B11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="220"/>
+      <c r="C11" s="223"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="221">
+      <c r="A12" s="224">
         <v>6</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="220"/>
+      <c r="C12" s="223"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="221"/>
+      <c r="A13" s="224"/>
       <c r="B13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="220"/>
+      <c r="C13" s="223"/>
     </row>
     <row r="14" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
@@ -5107,7 +5115,7 @@
       <c r="B14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="220"/>
+      <c r="C14" s="223"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
@@ -5116,7 +5124,7 @@
       <c r="B15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="220"/>
+      <c r="C15" s="223"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
@@ -5125,7 +5133,7 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="220"/>
+      <c r="C16" s="223"/>
     </row>
     <row r="17" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
@@ -5134,7 +5142,7 @@
       <c r="B17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="220"/>
+      <c r="C17" s="223"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -5149,7 +5157,7 @@
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" ht="82.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="218" t="s">
+      <c r="A20" s="221" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -5158,19 +5166,19 @@
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="218"/>
+      <c r="A21" s="221"/>
       <c r="B21" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" ht="0.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="218"/>
+      <c r="A22" s="221"/>
       <c r="B22" s="10"/>
       <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" ht="1.1499999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="218"/>
+      <c r="A23" s="221"/>
       <c r="B23" s="10"/>
       <c r="C23" s="8"/>
     </row>
@@ -5195,7 +5203,7 @@
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="218" t="s">
+      <c r="A28" s="221" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -5204,21 +5212,21 @@
       <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="218"/>
+      <c r="A29" s="221"/>
       <c r="B29" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="218"/>
+      <c r="A30" s="221"/>
       <c r="B30" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" ht="157.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="218"/>
+      <c r="A31" s="221"/>
       <c r="B31" s="10"/>
       <c r="C31" s="8"/>
     </row>
@@ -5256,21 +5264,21 @@
       <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="218" t="s">
+      <c r="A37" s="221" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="8"/>
     </row>
     <row r="38" spans="1:3" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="218"/>
+      <c r="A38" s="221"/>
       <c r="B38" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="218"/>
+      <c r="A39" s="221"/>
       <c r="B39" s="10"/>
       <c r="C39" s="8"/>
     </row>
@@ -5324,25 +5332,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="222" t="s">
+      <c r="A1" s="225" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="222"/>
-      <c r="C1" s="222"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="223" t="s">
+      <c r="A2" s="226" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="223"/>
+      <c r="B2" s="226"/>
       <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
+      <c r="A3" s="227" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
+      <c r="B3" s="227"/>
+      <c r="C3" s="227"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -5388,7 +5396,7 @@
       <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="225" t="s">
+      <c r="A9" s="228" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -5397,32 +5405,32 @@
       <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="225"/>
+      <c r="A10" s="228"/>
       <c r="B10" s="25"/>
       <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="225"/>
+      <c r="A11" s="228"/>
       <c r="B11" s="26"/>
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="225"/>
+      <c r="A12" s="228"/>
       <c r="B12" s="26"/>
       <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="225"/>
+      <c r="A13" s="228"/>
       <c r="B13" s="26"/>
       <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="225"/>
+      <c r="A14" s="228"/>
       <c r="B14" s="27"/>
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:3" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="225"/>
+      <c r="A15" s="228"/>
       <c r="B15" s="20"/>
       <c r="C15" s="8"/>
     </row>
@@ -5453,7 +5461,7 @@
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" ht="196.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="221">
+      <c r="A20" s="224">
         <v>8</v>
       </c>
       <c r="B20" s="20" t="s">
@@ -5462,19 +5470,19 @@
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="221"/>
+      <c r="A21" s="224"/>
       <c r="B21" s="24"/>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" ht="270" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="221"/>
+      <c r="A22" s="224"/>
       <c r="B22" s="20" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="221"/>
+      <c r="A23" s="224"/>
       <c r="B23" s="24"/>
       <c r="C23" s="8"/>
     </row>
@@ -5493,7 +5501,7 @@
       <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="221">
+      <c r="A26" s="224">
         <v>10</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -5502,19 +5510,19 @@
       <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="221"/>
+      <c r="A27" s="224"/>
       <c r="B27" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="221"/>
+      <c r="A28" s="224"/>
       <c r="B28" s="24"/>
       <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="221"/>
+      <c r="A29" s="224"/>
       <c r="B29" s="24"/>
       <c r="C29" s="8"/>
     </row>
@@ -5524,12 +5532,12 @@
       <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="221"/>
+      <c r="A31" s="224"/>
       <c r="B31" s="20"/>
       <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="221"/>
+      <c r="A32" s="224"/>
       <c r="B32" s="24"/>
       <c r="C32" s="8"/>
     </row>
@@ -5553,12 +5561,12 @@
       <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="221"/>
+      <c r="A36" s="224"/>
       <c r="B36" s="30"/>
       <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="221"/>
+      <c r="A37" s="224"/>
       <c r="B37" s="31" t="s">
         <v>50</v>
       </c>
@@ -5590,8 +5598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AR91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
+    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -5609,58 +5617,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="241"/>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
-      <c r="E1" s="241"/>
-      <c r="F1" s="241"/>
-      <c r="G1" s="241"/>
-      <c r="H1" s="241"/>
-      <c r="I1" s="241"/>
-      <c r="J1" s="241"/>
-      <c r="K1" s="241"/>
-      <c r="L1" s="241"/>
-      <c r="M1" s="241"/>
-      <c r="N1" s="241"/>
-      <c r="O1" s="241"/>
-      <c r="P1" s="241"/>
-      <c r="Q1" s="241"/>
-      <c r="R1" s="241"/>
-      <c r="S1" s="241"/>
-      <c r="T1" s="241"/>
-      <c r="U1" s="241"/>
-      <c r="V1" s="241"/>
-      <c r="W1" s="241"/>
-      <c r="X1" s="241"/>
-      <c r="Y1" s="241"/>
-      <c r="Z1" s="241"/>
-      <c r="AA1" s="241"/>
-      <c r="AB1" s="241"/>
-      <c r="AC1" s="241"/>
-      <c r="AD1" s="241"/>
-      <c r="AE1" s="241"/>
-      <c r="AF1" s="241"/>
-      <c r="AG1" s="241"/>
-      <c r="AH1" s="241"/>
-      <c r="AI1" s="241"/>
-      <c r="AJ1" s="241"/>
-      <c r="AK1" s="241"/>
-      <c r="AL1" s="241"/>
-      <c r="AM1" s="241"/>
-      <c r="AN1" s="241"/>
-      <c r="AO1" s="241"/>
-      <c r="AP1" s="241"/>
-      <c r="AQ1" s="241"/>
-      <c r="AR1" s="241"/>
+      <c r="A1" s="229"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
+      <c r="I1" s="229"/>
+      <c r="J1" s="229"/>
+      <c r="K1" s="229"/>
+      <c r="L1" s="229"/>
+      <c r="M1" s="229"/>
+      <c r="N1" s="229"/>
+      <c r="O1" s="229"/>
+      <c r="P1" s="229"/>
+      <c r="Q1" s="229"/>
+      <c r="R1" s="229"/>
+      <c r="S1" s="229"/>
+      <c r="T1" s="229"/>
+      <c r="U1" s="229"/>
+      <c r="V1" s="229"/>
+      <c r="W1" s="229"/>
+      <c r="X1" s="229"/>
+      <c r="Y1" s="229"/>
+      <c r="Z1" s="229"/>
+      <c r="AA1" s="229"/>
+      <c r="AB1" s="229"/>
+      <c r="AC1" s="229"/>
+      <c r="AD1" s="229"/>
+      <c r="AE1" s="229"/>
+      <c r="AF1" s="229"/>
+      <c r="AG1" s="229"/>
+      <c r="AH1" s="229"/>
+      <c r="AI1" s="229"/>
+      <c r="AJ1" s="229"/>
+      <c r="AK1" s="229"/>
+      <c r="AL1" s="229"/>
+      <c r="AM1" s="229"/>
+      <c r="AN1" s="229"/>
+      <c r="AO1" s="229"/>
+      <c r="AP1" s="229"/>
+      <c r="AQ1" s="229"/>
+      <c r="AR1" s="229"/>
     </row>
     <row r="2" spans="1:44" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="241"/>
-      <c r="B2" s="247" t="s">
+      <c r="A2" s="229"/>
+      <c r="B2" s="245" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="248"/>
-      <c r="D2" s="249"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="247"/>
       <c r="E2" s="33" t="s">
         <v>53</v>
       </c>
@@ -5677,7 +5685,7 @@
       <c r="J2" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="242" t="s">
+      <c r="K2" s="230" t="s">
         <v>58</v>
       </c>
       <c r="L2" s="38" t="s">
@@ -5686,17 +5694,17 @@
       <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="241"/>
-      <c r="B3" s="236" t="s">
+      <c r="A3" s="229"/>
+      <c r="B3" s="242" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="237"/>
-      <c r="D3" s="238"/>
-      <c r="E3" s="234">
+      <c r="C3" s="243"/>
+      <c r="D3" s="244"/>
+      <c r="E3" s="250">
         <f>SUM(E5:E27)</f>
         <v>1680</v>
       </c>
-      <c r="F3" s="231">
+      <c r="F3" s="248">
         <f>SUM(F5:F26)</f>
         <v>0</v>
       </c>
@@ -5713,7 +5721,7 @@
         <f>COUNTIF(C27, "Прочитал")/SUM(I8)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="243"/>
+      <c r="K3" s="231"/>
       <c r="L3" s="44">
         <f>ROUNDUP(E3/60, 0)</f>
         <v>28</v>
@@ -5721,7 +5729,7 @@
       <c r="M3" s="39"/>
     </row>
     <row r="4" spans="1:44" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="241"/>
+      <c r="A4" s="229"/>
       <c r="B4" s="45" t="s">
         <v>61</v>
       </c>
@@ -5731,42 +5739,42 @@
       <c r="D4" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="235"/>
-      <c r="F4" s="232"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="249"/>
       <c r="G4" s="35"/>
-      <c r="H4" s="245" t="s">
+      <c r="H4" s="233" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="246"/>
+      <c r="I4" s="234"/>
       <c r="J4" s="48">
         <f>COUNTIF(C6:C26, "Изучил")</f>
         <v>0</v>
       </c>
-      <c r="K4" s="243"/>
+      <c r="K4" s="231"/>
       <c r="L4" s="49" t="s">
         <v>65</v>
       </c>
       <c r="M4" s="39"/>
     </row>
     <row r="5" spans="1:44" ht="34.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="241"/>
-      <c r="B5" s="267" t="s">
+      <c r="A5" s="229"/>
+      <c r="B5" s="239" t="s">
         <v>330</v>
       </c>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="269"/>
+      <c r="C5" s="240"/>
+      <c r="D5" s="240"/>
+      <c r="E5" s="240"/>
+      <c r="F5" s="241"/>
       <c r="G5" s="35"/>
-      <c r="H5" s="226" t="s">
+      <c r="H5" s="235" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="227"/>
+      <c r="I5" s="236"/>
       <c r="J5" s="50">
         <f>COUNTIF(C6:C26, "Изучил")</f>
         <v>0</v>
       </c>
-      <c r="K5" s="244"/>
+      <c r="K5" s="232"/>
       <c r="L5" s="51">
         <f>ROUNDUP(F3/60, 0)</f>
         <v>0</v>
@@ -5774,7 +5782,7 @@
       <c r="M5" s="39"/>
     </row>
     <row r="6" spans="1:44" ht="51.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="241"/>
+      <c r="A6" s="229"/>
       <c r="B6" s="52" t="s">
         <v>67</v>
       </c>
@@ -5789,7 +5797,7 @@
       <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:44" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="241"/>
+      <c r="A7" s="229"/>
       <c r="B7" s="52" t="s">
         <v>69</v>
       </c>
@@ -5811,7 +5819,7 @@
       <c r="J7" s="39"/>
     </row>
     <row r="8" spans="1:44" ht="36" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="241"/>
+      <c r="A8" s="229"/>
       <c r="B8" s="58" t="s">
         <v>71</v>
       </c>
@@ -5832,7 +5840,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="241"/>
+      <c r="A9" s="229"/>
       <c r="B9" s="62" t="s">
         <v>73</v>
       </c>
@@ -5847,7 +5855,7 @@
       <c r="G9" s="35"/>
     </row>
     <row r="10" spans="1:44" ht="43.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="241"/>
+      <c r="A10" s="229"/>
       <c r="B10" s="63" t="s">
         <v>74</v>
       </c>
@@ -5860,16 +5868,16 @@
       </c>
       <c r="F10" s="55"/>
       <c r="G10" s="35"/>
-      <c r="H10" s="239" t="s">
+      <c r="H10" s="237" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="240"/>
+      <c r="I10" s="238"/>
       <c r="K10" s="64" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:44" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="241"/>
+      <c r="A11" s="229"/>
       <c r="B11" s="52" t="s">
         <v>77</v>
       </c>
@@ -5884,7 +5892,7 @@
       <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:44" ht="39" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="241"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="52" t="s">
         <v>78</v>
       </c>
@@ -5899,7 +5907,7 @@
       <c r="G12" s="35"/>
     </row>
     <row r="13" spans="1:44" ht="25.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="241"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="52" t="s">
         <v>79</v>
       </c>
@@ -5914,7 +5922,7 @@
       <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:44" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="241"/>
+      <c r="A14" s="229"/>
       <c r="B14" s="58" t="s">
         <v>80</v>
       </c>
@@ -5929,7 +5937,7 @@
       <c r="G14" s="35"/>
     </row>
     <row r="15" spans="1:44" ht="36" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="241"/>
+      <c r="A15" s="229"/>
       <c r="B15" s="63" t="s">
         <v>81</v>
       </c>
@@ -5944,7 +5952,7 @@
       <c r="G15" s="35"/>
     </row>
     <row r="16" spans="1:44" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="241"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="58" t="s">
         <v>82</v>
       </c>
@@ -5959,7 +5967,7 @@
       <c r="G16" s="35"/>
     </row>
     <row r="17" spans="1:12" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="241"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="63" t="s">
         <v>83</v>
       </c>
@@ -5974,7 +5982,7 @@
       <c r="G17" s="35"/>
     </row>
     <row r="18" spans="1:12" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="241"/>
+      <c r="A18" s="229"/>
       <c r="B18" s="58" t="s">
         <v>84</v>
       </c>
@@ -5989,7 +5997,7 @@
       <c r="G18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="241"/>
+      <c r="A19" s="229"/>
       <c r="B19" s="58" t="s">
         <v>85</v>
       </c>
@@ -6004,7 +6012,7 @@
       <c r="G19" s="35"/>
     </row>
     <row r="20" spans="1:12" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="241"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="63" t="s">
         <v>86</v>
       </c>
@@ -6019,7 +6027,7 @@
       <c r="G20" s="35"/>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="241"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="58" t="s">
         <v>87</v>
       </c>
@@ -6034,7 +6042,7 @@
       <c r="G21" s="35"/>
     </row>
     <row r="22" spans="1:12" ht="37.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="241"/>
+      <c r="A22" s="229"/>
       <c r="B22" s="63" t="s">
         <v>88</v>
       </c>
@@ -6049,7 +6057,7 @@
       <c r="G22" s="35"/>
     </row>
     <row r="23" spans="1:12" ht="25.9" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="241"/>
+      <c r="A23" s="229"/>
       <c r="B23" s="52" t="s">
         <v>89</v>
       </c>
@@ -6064,7 +6072,7 @@
       <c r="G23" s="35"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="241"/>
+      <c r="A24" s="229"/>
       <c r="B24" s="52" t="s">
         <v>90</v>
       </c>
@@ -6079,7 +6087,7 @@
       <c r="G24" s="35"/>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="241"/>
+      <c r="A25" s="229"/>
       <c r="B25" s="52" t="s">
         <v>91</v>
       </c>
@@ -6094,7 +6102,7 @@
       <c r="G25" s="35"/>
     </row>
     <row r="26" spans="1:12" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="241"/>
+      <c r="A26" s="229"/>
       <c r="B26" s="52" t="s">
         <v>92</v>
       </c>
@@ -6109,7 +6117,7 @@
       <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:12" ht="33" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="241"/>
+      <c r="A27" s="229"/>
       <c r="B27" s="71" t="s">
         <v>93</v>
       </c>
@@ -6123,7 +6131,7 @@
       <c r="F27" s="74"/>
     </row>
     <row r="28" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="241"/>
+      <c r="A28" s="229"/>
       <c r="B28" s="75"/>
       <c r="C28" s="75"/>
       <c r="D28" s="75"/>
@@ -6136,12 +6144,12 @@
       <c r="L28" s="77"/>
     </row>
     <row r="29" spans="1:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="241"/>
-      <c r="B29" s="252" t="s">
+      <c r="A29" s="229"/>
+      <c r="B29" s="254" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="248"/>
-      <c r="D29" s="253"/>
+      <c r="C29" s="246"/>
+      <c r="D29" s="255"/>
       <c r="E29" s="81" t="s">
         <v>53</v>
       </c>
@@ -6158,7 +6166,7 @@
       <c r="J29" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="K29" s="242" t="s">
+      <c r="K29" s="230" t="s">
         <v>58</v>
       </c>
       <c r="L29" s="38" t="s">
@@ -6166,17 +6174,17 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="241"/>
-      <c r="B30" s="236" t="s">
+      <c r="A30" s="229"/>
+      <c r="B30" s="242" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="237"/>
-      <c r="D30" s="238"/>
-      <c r="E30" s="234">
+      <c r="C30" s="243"/>
+      <c r="D30" s="244"/>
+      <c r="E30" s="250">
         <f>SUM(E32:E55)</f>
         <v>6750</v>
       </c>
-      <c r="F30" s="231">
+      <c r="F30" s="248">
         <f>SUM(F32:F38)</f>
         <v>0</v>
       </c>
@@ -6193,14 +6201,14 @@
         <f>COUNTIF(C39, "Прочитал")/SUM(I35)</f>
         <v>0</v>
       </c>
-      <c r="K30" s="243"/>
+      <c r="K30" s="231"/>
       <c r="L30" s="44">
         <f>ROUNDUP(E30/60, 0)</f>
         <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="241"/>
+      <c r="A31" s="229"/>
       <c r="B31" s="45" t="s">
         <v>61</v>
       </c>
@@ -6210,48 +6218,48 @@
       <c r="D31" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="235"/>
-      <c r="F31" s="232"/>
+      <c r="E31" s="251"/>
+      <c r="F31" s="249"/>
       <c r="G31" s="86"/>
-      <c r="H31" s="229" t="s">
+      <c r="H31" s="258" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="230"/>
+      <c r="I31" s="259"/>
       <c r="J31" s="87">
         <f>COUNTIF(C33:C38, "Решил")</f>
         <v>0</v>
       </c>
-      <c r="K31" s="243"/>
+      <c r="K31" s="231"/>
       <c r="L31" s="49" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="39" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="241"/>
-      <c r="B32" s="270" t="s">
+      <c r="A32" s="229"/>
+      <c r="B32" s="261" t="s">
         <v>331</v>
       </c>
-      <c r="C32" s="271"/>
-      <c r="D32" s="271"/>
-      <c r="E32" s="271"/>
-      <c r="F32" s="272"/>
+      <c r="C32" s="262"/>
+      <c r="D32" s="262"/>
+      <c r="E32" s="262"/>
+      <c r="F32" s="263"/>
       <c r="G32" s="86"/>
-      <c r="H32" s="226" t="s">
+      <c r="H32" s="235" t="s">
         <v>64</v>
       </c>
-      <c r="I32" s="227"/>
+      <c r="I32" s="236"/>
       <c r="J32" s="88">
         <f>COUNTIF(C33:C38, "Решил")</f>
         <v>0</v>
       </c>
-      <c r="K32" s="244"/>
+      <c r="K32" s="232"/>
       <c r="L32" s="51">
         <f>ROUNDUP(F30/60, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="26.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="241"/>
+      <c r="A33" s="229"/>
       <c r="B33" s="89" t="s">
         <v>98</v>
       </c>
@@ -6267,7 +6275,7 @@
       <c r="H33" s="92"/>
     </row>
     <row r="34" spans="1:10" ht="34.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="241"/>
+      <c r="A34" s="229"/>
       <c r="B34" s="93" t="s">
         <v>100</v>
       </c>
@@ -6289,7 +6297,7 @@
       <c r="J34" s="96"/>
     </row>
     <row r="35" spans="1:10" ht="26.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="241"/>
+      <c r="A35" s="229"/>
       <c r="B35" s="97" t="s">
         <v>102</v>
       </c>
@@ -6310,7 +6318,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="22.9" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="241"/>
+      <c r="A36" s="229"/>
       <c r="B36" s="97" t="s">
         <v>103</v>
       </c>
@@ -6327,7 +6335,7 @@
       <c r="I36" s="98"/>
     </row>
     <row r="37" spans="1:10" ht="32.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="241"/>
+      <c r="A37" s="229"/>
       <c r="B37" s="93" t="s">
         <v>104</v>
       </c>
@@ -6340,13 +6348,13 @@
       </c>
       <c r="F37" s="90"/>
       <c r="G37" s="91"/>
-      <c r="H37" s="239" t="s">
+      <c r="H37" s="237" t="s">
         <v>75</v>
       </c>
-      <c r="I37" s="240"/>
+      <c r="I37" s="238"/>
     </row>
     <row r="38" spans="1:10" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="241"/>
+      <c r="A38" s="229"/>
       <c r="B38" s="99" t="s">
         <v>105</v>
       </c>
@@ -6360,8 +6368,8 @@
       <c r="F38" s="100"/>
     </row>
     <row r="39" spans="1:10" ht="37.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="241"/>
-      <c r="B39" s="262" t="s">
+      <c r="A39" s="229"/>
+      <c r="B39" s="218" t="s">
         <v>106</v>
       </c>
       <c r="C39" s="72" t="s">
@@ -6374,95 +6382,95 @@
       <c r="F39" s="100"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="241"/>
+      <c r="A40" s="229"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="241"/>
+      <c r="A41" s="229"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="241"/>
+      <c r="A42" s="229"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="241"/>
+      <c r="A43" s="229"/>
       <c r="H43" s="98"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="241"/>
+      <c r="A44" s="229"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="241"/>
+      <c r="A45" s="229"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="241"/>
+      <c r="A46" s="229"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="241"/>
+      <c r="A47" s="229"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="241"/>
+      <c r="A48" s="229"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="241"/>
-      <c r="B49" s="250"/>
-      <c r="C49" s="250"/>
-      <c r="D49" s="250"/>
+      <c r="A49" s="229"/>
+      <c r="B49" s="252"/>
+      <c r="C49" s="252"/>
+      <c r="D49" s="252"/>
       <c r="E49" s="102"/>
       <c r="F49" s="103"/>
       <c r="G49" s="98"/>
       <c r="H49" s="103"/>
       <c r="I49" s="103"/>
       <c r="J49" s="103"/>
-      <c r="K49" s="254"/>
+      <c r="K49" s="256"/>
       <c r="L49" s="103"/>
       <c r="M49" s="98"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="241"/>
-      <c r="B50" s="251"/>
-      <c r="C50" s="251"/>
-      <c r="D50" s="251"/>
-      <c r="E50" s="220"/>
-      <c r="F50" s="220"/>
+      <c r="A50" s="229"/>
+      <c r="B50" s="253"/>
+      <c r="C50" s="253"/>
+      <c r="D50" s="253"/>
+      <c r="E50" s="223"/>
+      <c r="F50" s="223"/>
       <c r="G50" s="98"/>
       <c r="H50" s="104"/>
       <c r="I50" s="104"/>
       <c r="J50" s="104"/>
-      <c r="K50" s="254"/>
+      <c r="K50" s="256"/>
       <c r="L50" s="101"/>
       <c r="M50" s="98"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="241"/>
+      <c r="A51" s="229"/>
       <c r="B51" s="8"/>
       <c r="C51" s="102"/>
       <c r="D51" s="102"/>
-      <c r="E51" s="220"/>
-      <c r="F51" s="220"/>
+      <c r="E51" s="223"/>
+      <c r="F51" s="223"/>
       <c r="G51" s="98"/>
-      <c r="H51" s="228"/>
-      <c r="I51" s="228"/>
+      <c r="H51" s="257"/>
+      <c r="I51" s="257"/>
       <c r="J51" s="105"/>
-      <c r="K51" s="254"/>
+      <c r="K51" s="256"/>
       <c r="L51" s="103"/>
       <c r="M51" s="98"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="241"/>
-      <c r="B52" s="233"/>
-      <c r="C52" s="233"/>
-      <c r="D52" s="233"/>
-      <c r="E52" s="233"/>
-      <c r="F52" s="233"/>
+      <c r="A52" s="229"/>
+      <c r="B52" s="260"/>
+      <c r="C52" s="260"/>
+      <c r="D52" s="260"/>
+      <c r="E52" s="260"/>
+      <c r="F52" s="260"/>
       <c r="G52" s="98"/>
-      <c r="H52" s="228"/>
-      <c r="I52" s="228"/>
+      <c r="H52" s="257"/>
+      <c r="I52" s="257"/>
       <c r="J52" s="105"/>
-      <c r="K52" s="254"/>
+      <c r="K52" s="256"/>
       <c r="L52" s="101"/>
       <c r="M52" s="98"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="241"/>
+      <c r="A53" s="229"/>
       <c r="B53" s="106"/>
       <c r="C53" s="107"/>
       <c r="D53" s="108"/>
@@ -6477,7 +6485,7 @@
       <c r="M53" s="98"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="241"/>
+      <c r="A54" s="229"/>
       <c r="B54" s="106"/>
       <c r="C54" s="107"/>
       <c r="D54" s="108"/>
@@ -6492,7 +6500,7 @@
       <c r="M54" s="98"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="241"/>
+      <c r="A55" s="229"/>
       <c r="B55" s="106"/>
       <c r="C55" s="107"/>
       <c r="D55" s="108"/>
@@ -6507,7 +6515,7 @@
       <c r="M55" s="98"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="241"/>
+      <c r="A56" s="229"/>
       <c r="B56" s="106"/>
       <c r="C56" s="107"/>
       <c r="D56" s="108"/>
@@ -6522,7 +6530,7 @@
       <c r="M56" s="98"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="241"/>
+      <c r="A57" s="229"/>
       <c r="B57" s="106"/>
       <c r="C57" s="107"/>
       <c r="D57" s="108"/>
@@ -6537,7 +6545,7 @@
       <c r="M57" s="98"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="241"/>
+      <c r="A58" s="229"/>
       <c r="B58" s="106"/>
       <c r="C58" s="107"/>
       <c r="D58" s="108"/>
@@ -6552,106 +6560,118 @@
       <c r="M58" s="98"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="241"/>
+      <c r="A59" s="229"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="241"/>
+      <c r="A60" s="229"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="241"/>
+      <c r="A61" s="229"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="241"/>
+      <c r="A62" s="229"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="241"/>
+      <c r="A63" s="229"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="241"/>
+      <c r="A64" s="229"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="241"/>
+      <c r="A65" s="229"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="241"/>
+      <c r="A66" s="229"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="241"/>
+      <c r="A67" s="229"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="241"/>
+      <c r="A68" s="229"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="241"/>
+      <c r="A69" s="229"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="241"/>
+      <c r="A70" s="229"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="241"/>
+      <c r="A71" s="229"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="241"/>
+      <c r="A72" s="229"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="241"/>
+      <c r="A73" s="229"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="241"/>
+      <c r="A74" s="229"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="241"/>
+      <c r="A75" s="229"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="241"/>
+      <c r="A76" s="229"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="241"/>
+      <c r="A77" s="229"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="241"/>
+      <c r="A78" s="229"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="241"/>
+      <c r="A79" s="229"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="241"/>
+      <c r="A80" s="229"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="241"/>
+      <c r="A81" s="229"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="241"/>
+      <c r="A82" s="229"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="241"/>
+      <c r="A83" s="229"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="241"/>
+      <c r="A84" s="229"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="241"/>
+      <c r="A85" s="229"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="241"/>
+      <c r="A86" s="229"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="241"/>
+      <c r="A87" s="229"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="241"/>
+      <c r="A88" s="229"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="241"/>
+      <c r="A89" s="229"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="241"/>
+      <c r="A90" s="229"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="241"/>
+      <c r="A91" s="229"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="H37:I37"/>
     <mergeCell ref="A1:AR1"/>
     <mergeCell ref="K2:K5"/>
     <mergeCell ref="H4:I4"/>
@@ -6668,18 +6688,6 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="K49:K52"/>
     <mergeCell ref="K29:K32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="H37:I37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B27" r:id="rId1" display="https://disk.yandex.ru/i/Y5t__LB6BFXs8Q" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -6701,13 +6709,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:L59"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="75.28515625" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
@@ -6720,11 +6728,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="252" t="s">
+      <c r="B2" s="254" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="248"/>
-      <c r="D2" s="253"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="255"/>
       <c r="E2" s="33" t="s">
         <v>53</v>
       </c>
@@ -6740,7 +6748,7 @@
       <c r="J2" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="242" t="s">
+      <c r="K2" s="230" t="s">
         <v>58</v>
       </c>
       <c r="L2" s="116" t="s">
@@ -6753,11 +6761,11 @@
       </c>
       <c r="C3" s="118"/>
       <c r="D3" s="119"/>
-      <c r="E3" s="231">
+      <c r="E3" s="248">
         <f>SUM(E5:E58)</f>
         <v>4550</v>
       </c>
-      <c r="F3" s="231">
+      <c r="F3" s="248">
         <f>SUM(F5:F57)</f>
         <v>0</v>
       </c>
@@ -6773,7 +6781,7 @@
         <f>COUNTIF(C58, "Прочитал")/SUM(I9)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="243"/>
+      <c r="K3" s="231"/>
       <c r="L3" s="123">
         <f>ROUNDUP(E3/60, 0)</f>
         <v>76</v>
@@ -6789,38 +6797,38 @@
       <c r="D4" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="232"/>
-      <c r="F4" s="232"/>
-      <c r="H4" s="245" t="s">
+      <c r="E4" s="249"/>
+      <c r="F4" s="249"/>
+      <c r="H4" s="233" t="s">
         <v>111</v>
       </c>
-      <c r="I4" s="246"/>
+      <c r="I4" s="234"/>
       <c r="J4" s="48">
         <f>COUNTIF(C6:C56, "Изучил")</f>
         <v>0</v>
       </c>
-      <c r="K4" s="243"/>
+      <c r="K4" s="231"/>
       <c r="L4" s="125" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="273" t="s">
+      <c r="B5" s="264" t="s">
         <v>332</v>
       </c>
-      <c r="C5" s="274"/>
-      <c r="D5" s="274"/>
-      <c r="E5" s="274"/>
-      <c r="F5" s="275"/>
-      <c r="H5" s="226" t="s">
+      <c r="C5" s="265"/>
+      <c r="D5" s="265"/>
+      <c r="E5" s="265"/>
+      <c r="F5" s="266"/>
+      <c r="H5" s="235" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="227"/>
+      <c r="I5" s="236"/>
       <c r="J5" s="126">
         <f>COUNTIF(C7:C57, "Решил")</f>
         <v>0</v>
       </c>
-      <c r="K5" s="244"/>
+      <c r="K5" s="232"/>
       <c r="L5" s="127">
         <f>ROUNDUP(F3/60, 0)</f>
         <v>0</v>
@@ -6925,10 +6933,10 @@
         <v>25</v>
       </c>
       <c r="F11" s="129"/>
-      <c r="H11" s="239" t="s">
+      <c r="H11" s="237" t="s">
         <v>121</v>
       </c>
-      <c r="I11" s="240"/>
+      <c r="I11" s="238"/>
     </row>
     <row r="12" spans="2:12" ht="25.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12" s="138" t="s">
@@ -7529,7 +7537,7 @@
       <c r="F57" s="149"/>
     </row>
     <row r="58" spans="2:6" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="263" t="s">
+      <c r="B58" s="219" t="s">
         <v>168</v>
       </c>
       <c r="C58" s="72" t="s">
@@ -7595,8 +7603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7612,11 +7620,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="247" t="s">
+      <c r="B2" s="245" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="248"/>
-      <c r="D2" s="249"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="247"/>
       <c r="E2" s="46" t="s">
         <v>53</v>
       </c>
@@ -7632,7 +7640,7 @@
       <c r="J2" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="242" t="s">
+      <c r="K2" s="230" t="s">
         <v>58</v>
       </c>
       <c r="L2" s="116" t="s">
@@ -7640,16 +7648,16 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="236" t="s">
+      <c r="B3" s="242" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="237"/>
-      <c r="D3" s="238"/>
-      <c r="E3" s="234">
+      <c r="C3" s="243"/>
+      <c r="D3" s="244"/>
+      <c r="E3" s="250">
         <f>SUM(E6:E11)</f>
         <v>5760</v>
       </c>
-      <c r="F3" s="231">
+      <c r="F3" s="248">
         <f>SUM(F5:F10)</f>
         <v>0</v>
       </c>
@@ -7665,7 +7673,7 @@
         <f>COUNTIF(C11, "Прочитал")/SUM(I8)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="243"/>
+      <c r="K3" s="231"/>
       <c r="L3" s="123">
         <f>ROUNDUP(E3/60, 0)</f>
         <v>96</v>
@@ -7681,38 +7689,38 @@
       <c r="D4" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="235"/>
-      <c r="F4" s="232"/>
-      <c r="H4" s="245" t="s">
+      <c r="E4" s="251"/>
+      <c r="F4" s="249"/>
+      <c r="H4" s="233" t="s">
         <v>111</v>
       </c>
-      <c r="I4" s="246"/>
+      <c r="I4" s="234"/>
       <c r="J4" s="48">
         <f>COUNTIF(C6:C10, "Решил")</f>
         <v>0</v>
       </c>
-      <c r="K4" s="243"/>
+      <c r="K4" s="231"/>
       <c r="L4" s="125" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="21.6" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="255" t="s">
+      <c r="B5" s="267" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="256"/>
-      <c r="D5" s="256"/>
-      <c r="E5" s="256"/>
-      <c r="F5" s="257"/>
-      <c r="H5" s="226" t="s">
+      <c r="C5" s="268"/>
+      <c r="D5" s="268"/>
+      <c r="E5" s="268"/>
+      <c r="F5" s="269"/>
+      <c r="H5" s="235" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="227"/>
+      <c r="I5" s="236"/>
       <c r="J5" s="126">
         <f>COUNTIF(C6:C10, "Решил")</f>
         <v>0</v>
       </c>
-      <c r="K5" s="244"/>
+      <c r="K5" s="232"/>
       <c r="L5" s="127">
         <f>ROUNDUP(F3/60, 0)</f>
         <v>0</v>
@@ -7799,13 +7807,13 @@
       </c>
       <c r="F10" s="163"/>
       <c r="G10" s="96"/>
-      <c r="H10" s="265" t="s">
+      <c r="H10" s="270" t="s">
         <v>177</v>
       </c>
-      <c r="I10" s="266"/>
+      <c r="I10" s="271"/>
     </row>
     <row r="11" spans="2:12" ht="25.9" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="264" t="s">
+      <c r="B11" s="220" t="s">
         <v>178</v>
       </c>
       <c r="C11" s="72" t="s">
@@ -7858,32 +7866,32 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="165"/>
       <c r="B1" s="165"/>
-      <c r="C1" s="260" t="s">
+      <c r="C1" s="274" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
     </row>
     <row r="2" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="261" t="s">
+      <c r="B2" s="275" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="261"/>
-      <c r="D2" s="261"/>
-      <c r="E2" s="261"/>
-      <c r="F2" s="261"/>
-      <c r="G2" s="261"/>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261"/>
-      <c r="J2" s="261"/>
-      <c r="K2" s="261"/>
+      <c r="C2" s="275"/>
+      <c r="D2" s="275"/>
+      <c r="E2" s="275"/>
+      <c r="F2" s="275"/>
+      <c r="G2" s="275"/>
+      <c r="H2" s="275"/>
+      <c r="I2" s="275"/>
+      <c r="J2" s="275"/>
+      <c r="K2" s="275"/>
     </row>
     <row r="3" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
@@ -7919,7 +7927,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="258" t="s">
+      <c r="A4" s="272" t="s">
         <v>192</v>
       </c>
       <c r="B4" s="175" t="str">
@@ -7964,7 +7972,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="259"/>
+      <c r="A5" s="273"/>
       <c r="B5" s="184" t="str">
         <f>'План на 1 месяц'!B29:D29</f>
         <v xml:space="preserve">БЛОК 2 "Практика" </v>
@@ -8007,7 +8015,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="258" t="s">
+      <c r="A6" s="272" t="s">
         <v>193</v>
       </c>
       <c r="B6" s="184" t="str">
@@ -8052,7 +8060,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="259"/>
+      <c r="A7" s="273"/>
       <c r="B7" s="194" t="str">
         <f>'План на 3 месяц'!B2:D2</f>
         <v xml:space="preserve">БЛОК 4 "Практика" </v>
@@ -8263,7 +8271,7 @@
       </c>
       <c r="C2" s="215">
         <f ca="1">NOW()</f>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D2" s="213"/>
       <c r="E2" s="212"/>
@@ -8402,7 +8410,7 @@
       </c>
       <c r="C2" s="216">
         <f ca="1">NOW()</f>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8417,7 +8425,7 @@
       </c>
       <c r="C3" s="216">
         <f ca="1">NOW()</f>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -8432,7 +8440,7 @@
       </c>
       <c r="C4" s="216">
         <f ca="1">NOW()</f>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -8447,7 +8455,7 @@
       </c>
       <c r="C5" s="216">
         <f ca="1">NOW()</f>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -8501,7 +8509,7 @@
       </c>
       <c r="C2" s="216">
         <f t="shared" ref="C2:C33" ca="1" si="0">NOW()</f>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -8516,7 +8524,7 @@
       </c>
       <c r="C3" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -8531,7 +8539,7 @@
       </c>
       <c r="C4" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -8546,7 +8554,7 @@
       </c>
       <c r="C5" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -8561,7 +8569,7 @@
       </c>
       <c r="C6" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -8576,7 +8584,7 @@
       </c>
       <c r="C7" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -8591,7 +8599,7 @@
       </c>
       <c r="C8" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D8">
         <v>60</v>
@@ -8606,7 +8614,7 @@
       </c>
       <c r="C9" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D9">
         <v>60</v>
@@ -8621,7 +8629,7 @@
       </c>
       <c r="C10" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -8636,7 +8644,7 @@
       </c>
       <c r="C11" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D11">
         <v>60</v>
@@ -8651,7 +8659,7 @@
       </c>
       <c r="C12" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -8666,7 +8674,7 @@
       </c>
       <c r="C13" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D13">
         <v>60</v>
@@ -8681,7 +8689,7 @@
       </c>
       <c r="C14" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D14">
         <v>60</v>
@@ -8696,7 +8704,7 @@
       </c>
       <c r="C15" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D15">
         <v>60</v>
@@ -8711,7 +8719,7 @@
       </c>
       <c r="C16" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D16">
         <v>60</v>
@@ -8726,7 +8734,7 @@
       </c>
       <c r="C17" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D17">
         <v>60</v>
@@ -8741,7 +8749,7 @@
       </c>
       <c r="C18" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D18">
         <v>60</v>
@@ -8756,7 +8764,7 @@
       </c>
       <c r="C19" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D19">
         <v>60</v>
@@ -8771,7 +8779,7 @@
       </c>
       <c r="C20" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D20">
         <v>60</v>
@@ -8786,7 +8794,7 @@
       </c>
       <c r="C21" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D21">
         <v>60</v>
@@ -8801,7 +8809,7 @@
       </c>
       <c r="C22" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D22">
         <v>60</v>
@@ -8817,7 +8825,7 @@
       </c>
       <c r="C23" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D23">
         <v>1035</v>
@@ -8832,7 +8840,7 @@
       </c>
       <c r="C24" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D24">
         <v>1320</v>
@@ -8847,7 +8855,7 @@
       </c>
       <c r="C25" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D25">
         <v>1200</v>
@@ -8862,7 +8870,7 @@
       </c>
       <c r="C26" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D26">
         <v>1140</v>
@@ -8877,7 +8885,7 @@
       </c>
       <c r="C27" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D27">
         <v>900</v>
@@ -8892,7 +8900,7 @@
       </c>
       <c r="C28" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D28">
         <v>675</v>
@@ -8907,7 +8915,7 @@
       </c>
       <c r="C29" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D29">
         <v>15</v>
@@ -8922,7 +8930,7 @@
       </c>
       <c r="C30" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -8940,7 +8948,7 @@
       </c>
       <c r="C31" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D31">
         <v>40</v>
@@ -8955,7 +8963,7 @@
       </c>
       <c r="C32" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D32">
         <v>20</v>
@@ -8973,7 +8981,7 @@
       </c>
       <c r="C33" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D33">
         <v>45</v>
@@ -8988,7 +8996,7 @@
       </c>
       <c r="C34" s="216">
         <f t="shared" ref="C34:C65" ca="1" si="1">NOW()</f>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D34">
         <v>25</v>
@@ -9006,7 +9014,7 @@
       </c>
       <c r="C35" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D35">
         <v>130</v>
@@ -9021,7 +9029,7 @@
       </c>
       <c r="C36" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D36">
         <v>120</v>
@@ -9039,7 +9047,7 @@
       </c>
       <c r="C37" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D37">
         <v>90</v>
@@ -9054,7 +9062,7 @@
       </c>
       <c r="C38" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D38">
         <v>60</v>
@@ -9072,7 +9080,7 @@
       </c>
       <c r="C39" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D39">
         <v>120</v>
@@ -9087,7 +9095,7 @@
       </c>
       <c r="C40" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D40">
         <v>5</v>
@@ -9105,7 +9113,7 @@
       </c>
       <c r="C41" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D41">
         <v>50</v>
@@ -9120,7 +9128,7 @@
       </c>
       <c r="C42" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D42">
         <v>25</v>
@@ -9138,7 +9146,7 @@
       </c>
       <c r="C43" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D43">
         <v>25</v>
@@ -9153,7 +9161,7 @@
       </c>
       <c r="C44" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D44">
         <v>15</v>
@@ -9171,7 +9179,7 @@
       </c>
       <c r="C45" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D45">
         <v>40</v>
@@ -9186,7 +9194,7 @@
       </c>
       <c r="C46" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D46">
         <v>25</v>
@@ -9204,7 +9212,7 @@
       </c>
       <c r="C47" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D47">
         <v>50</v>
@@ -9219,7 +9227,7 @@
       </c>
       <c r="C48" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D48">
         <v>25</v>
@@ -9237,7 +9245,7 @@
       </c>
       <c r="C49" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D49">
         <v>40</v>
@@ -9252,7 +9260,7 @@
       </c>
       <c r="C50" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D50">
         <v>25</v>
@@ -9270,7 +9278,7 @@
       </c>
       <c r="C51" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D51">
         <v>80</v>
@@ -9285,7 +9293,7 @@
       </c>
       <c r="C52" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D52">
         <v>40</v>
@@ -9303,7 +9311,7 @@
       </c>
       <c r="C53" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D53">
         <v>40</v>
@@ -9318,7 +9326,7 @@
       </c>
       <c r="C54" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D54">
         <v>25</v>
@@ -9336,7 +9344,7 @@
       </c>
       <c r="C55" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D55">
         <v>270</v>
@@ -9351,7 +9359,7 @@
       </c>
       <c r="C56" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D56">
         <v>90</v>
@@ -9369,7 +9377,7 @@
       </c>
       <c r="C57" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D57">
         <v>210</v>
@@ -9384,7 +9392,7 @@
       </c>
       <c r="C58" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D58">
         <v>90</v>
@@ -9402,7 +9410,7 @@
       </c>
       <c r="C59" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D59">
         <v>170</v>
@@ -9417,7 +9425,7 @@
       </c>
       <c r="C60" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D60">
         <v>5</v>
@@ -9435,7 +9443,7 @@
       </c>
       <c r="C61" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D61">
         <v>40</v>
@@ -9450,7 +9458,7 @@
       </c>
       <c r="C62" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D62">
         <v>5</v>
@@ -9468,7 +9476,7 @@
       </c>
       <c r="C63" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D63">
         <v>35</v>
@@ -9483,7 +9491,7 @@
       </c>
       <c r="C64" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D64">
         <v>90</v>
@@ -9501,7 +9509,7 @@
       </c>
       <c r="C65" s="216">
         <f t="shared" ca="1" si="1"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D65">
         <v>40</v>
@@ -9516,7 +9524,7 @@
       </c>
       <c r="C66" s="216">
         <f t="shared" ref="C66:C85" ca="1" si="2">NOW()</f>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D66">
         <v>25</v>
@@ -9534,7 +9542,7 @@
       </c>
       <c r="C67" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D67">
         <v>110</v>
@@ -9549,7 +9557,7 @@
       </c>
       <c r="C68" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D68">
         <v>120</v>
@@ -9567,7 +9575,7 @@
       </c>
       <c r="C69" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D69">
         <v>70</v>
@@ -9582,7 +9590,7 @@
       </c>
       <c r="C70" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D70">
         <v>50</v>
@@ -9600,7 +9608,7 @@
       </c>
       <c r="C71" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D71">
         <v>370</v>
@@ -9615,7 +9623,7 @@
       </c>
       <c r="C72" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D72">
         <v>180</v>
@@ -9633,7 +9641,7 @@
       </c>
       <c r="C73" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D73">
         <v>30</v>
@@ -9648,7 +9656,7 @@
       </c>
       <c r="C74" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D74">
         <v>25</v>
@@ -9666,7 +9674,7 @@
       </c>
       <c r="C75" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D75">
         <v>120</v>
@@ -9681,7 +9689,7 @@
       </c>
       <c r="C76" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D76">
         <v>5</v>
@@ -9699,7 +9707,7 @@
       </c>
       <c r="C77" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D77">
         <v>130</v>
@@ -9714,7 +9722,7 @@
       </c>
       <c r="C78" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D78">
         <v>5</v>
@@ -9732,7 +9740,7 @@
       </c>
       <c r="C79" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D79">
         <v>120</v>
@@ -9747,7 +9755,7 @@
       </c>
       <c r="C80" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D80">
         <v>5</v>
@@ -9765,7 +9773,7 @@
       </c>
       <c r="C81" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D81">
         <v>480</v>
@@ -9783,7 +9791,7 @@
       </c>
       <c r="C82" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D82">
         <v>960</v>
@@ -9801,7 +9809,7 @@
       </c>
       <c r="C83" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D83">
         <v>960</v>
@@ -9819,7 +9827,7 @@
       </c>
       <c r="C84" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D84">
         <v>1920</v>
@@ -9837,7 +9845,7 @@
       </c>
       <c r="C85" s="216">
         <f t="shared" ca="1" si="2"/>
-        <v>45746.897011458335</v>
+        <v>45747.458126273152</v>
       </c>
       <c r="D85">
         <v>1440</v>

</xml_diff>